<commit_message>
I don't know, lots of things.
</commit_message>
<xml_diff>
--- a/final_tables_4.24.17.xlsx
+++ b/final_tables_4.24.17.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7305" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7305" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="166">
   <si>
     <t>95% CI</t>
   </si>
@@ -264,9 +264,6 @@
   </si>
   <si>
     <t>Income (% FPL)</t>
-  </si>
-  <si>
-    <t>Short Sleep (&lt;6 hours per night)</t>
   </si>
   <si>
     <t>Poor sleep</t>
@@ -595,6 +592,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -690,7 +690,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -734,6 +734,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -755,11 +764,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1034,7 +1043,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1042,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K49" sqref="K49"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1058,37 +1067,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:9" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21" t="s">
+      <c r="D2" s="24"/>
+      <c r="E2" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21" t="s">
+      <c r="F2" s="24"/>
+      <c r="G2" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="21"/>
-    </row>
-    <row r="3" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>83</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>84</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>70</v>
@@ -1110,1192 +1119,1123 @@
       </c>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="32">
+        <v>16654</v>
+      </c>
+      <c r="D4" s="16">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f>table1_calc!B33</f>
+        <v>7322</v>
+      </c>
+      <c r="F4" s="8">
+        <f>table1_calc!C33</f>
+        <v>0.50246901349449935</v>
+      </c>
+      <c r="G4">
+        <f>table1_calc!B35</f>
+        <v>2593</v>
+      </c>
+      <c r="H4" s="8">
+        <f>table1_calc!C35</f>
+        <v>0.13802529458084356</v>
+      </c>
+      <c r="I4" s="12"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5">
+        <v>45.4</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="C4">
-        <v>45.4</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="E4">
+      <c r="E5">
         <v>45.2</v>
       </c>
-      <c r="F4" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="G4" s="3">
+      <c r="F5" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="G5" s="3">
         <v>45.1</v>
       </c>
-      <c r="H4" s="18" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.16944000000000001</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.202927</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="G5" s="19">
-        <v>0.17585000000000001</v>
-      </c>
       <c r="H5" s="18" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.16944000000000001</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.202927</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="G6" s="19">
+        <v>0.17585000000000001</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="9"/>
-    </row>
-    <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B7" t="str">
+      <c r="C7" s="5"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B8" t="str">
         <f>table1_calc!D2</f>
         <v>9-11th Grade (Includes 12th grade with no diploma)</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <f>table1_calc!B2</f>
         <v>2629</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D8" s="8">
         <f>table1_calc!C2</f>
         <v>0.12486114311188579</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <f>table1_calc!E2</f>
         <v>502</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F8" s="8">
         <f>table1_calc!F2</f>
         <v>0.43274066904212471</v>
       </c>
-      <c r="G7">
+      <c r="G8">
         <f>table1_calc!G2</f>
         <v>1185</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H8" s="8">
         <f>table1_calc!H2</f>
         <v>0.16353579652259004</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B8" t="str">
+    <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B9" t="str">
         <f>table1_calc!D3</f>
         <v>College Graduate or above</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <f>table1_calc!B3</f>
         <v>3135</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D9" s="8">
         <f>table1_calc!C3</f>
         <v>0.26255386707176359</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <f>table1_calc!E3</f>
         <v>319</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F9" s="8">
         <f>table1_calc!F3</f>
         <v>0.47693075157477455</v>
       </c>
-      <c r="G8">
+      <c r="G9">
         <f>table1_calc!G3</f>
         <v>1419</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H9" s="8">
         <f>table1_calc!H3</f>
         <v>7.692342920565258E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B9" t="str">
+    <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B10" t="str">
         <f>table1_calc!D4</f>
         <v>High School Grad/GED or Equivalent</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <f>table1_calc!B4</f>
         <v>3840</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D10" s="8">
         <f>table1_calc!C4</f>
         <v>0.24490627733231407</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <f>table1_calc!E4</f>
         <v>672</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F10" s="8">
         <f>table1_calc!F4</f>
         <v>0.26189816929697757</v>
       </c>
-      <c r="G9">
+      <c r="G10">
         <f>table1_calc!G4</f>
         <v>1830</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H10" s="8">
         <f>table1_calc!H4</f>
         <v>7.7853288514700261E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B10" t="str">
+    <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B11" t="str">
         <f>table1_calc!D5</f>
         <v>Less Than 9th Grade</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <f>table1_calc!B5</f>
         <v>2059</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D11" s="8">
         <f>table1_calc!C5</f>
         <v>6.5981532577349761E-2</v>
       </c>
-      <c r="E10">
+      <c r="E11">
         <f>table1_calc!E5</f>
         <v>356</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F11" s="8">
         <f>table1_calc!F5</f>
         <v>0.93827655253373843</v>
       </c>
-      <c r="G10">
+      <c r="G11">
         <f>table1_calc!G5</f>
         <v>841</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H11" s="8">
         <f>table1_calc!H5</f>
         <v>0.35136132907319062</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B11" t="str">
+    <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B12" t="str">
         <f>table1_calc!D6</f>
         <v>Some College or AA degree</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <f>table1_calc!B6</f>
         <v>4382</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D12" s="8">
         <f>table1_calc!C6</f>
         <v>0.30169717990668754</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <f>table1_calc!E6</f>
         <v>739</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F12" s="8">
         <f>table1_calc!F6</f>
         <v>0.22278046231375273</v>
       </c>
-      <c r="G11">
+      <c r="G12">
         <f>table1_calc!G6</f>
         <v>2040</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H12" s="8">
         <f>table1_calc!H6</f>
         <v>6.4637022887462092E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B13" t="str">
+    <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B14" t="str">
         <f>table1_calc!D7</f>
         <v>Female</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <f>table1_calc!B7</f>
         <v>8073</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D14" s="8">
         <f>table1_calc!C7</f>
         <v>0.51176271206351009</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <f>table1_calc!E7</f>
         <v>1297</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F14" s="8">
         <f>table1_calc!F7</f>
         <v>0.1442547675554102</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <f>table1_calc!G7</f>
         <v>3840</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H14" s="8">
         <f>table1_calc!H7</f>
         <v>3.7312066034715763E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B14" t="str">
+    <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B15" t="str">
         <f>table1_calc!D8</f>
         <v>Male</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <f>table1_calc!B8</f>
         <v>7999</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D15" s="8">
         <f>table1_calc!C8</f>
         <v>0.48823728793649079</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <f>table1_calc!E8</f>
         <v>1296</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F15" s="8">
         <f>table1_calc!F8</f>
         <v>0.14555300154929787</v>
       </c>
-      <c r="G14">
+      <c r="G15">
         <f>table1_calc!G8</f>
         <v>3482</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H15" s="8">
         <f>table1_calc!H8</f>
         <v>4.2651344716308E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B16" t="str">
+    <row r="17" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B17" t="str">
         <f>table1_calc!D9</f>
         <v>Mexican American</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <f>table1_calc!B9</f>
         <v>2895</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D17" s="8">
         <f>table1_calc!C9</f>
         <v>8.1401054607111875E-2</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <f>table1_calc!E9</f>
         <v>377</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F17" s="8">
         <f>table1_calc!F9</f>
         <v>1.0132250682125767</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <f>table1_calc!G9</f>
         <v>1166</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H17" s="8">
         <f>table1_calc!H9</f>
         <v>0.29760454605550918</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B17" t="str">
+    <row r="18" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B18" t="str">
         <f>table1_calc!D10</f>
         <v>Non-Hispanic Black</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <f>table1_calc!B10</f>
         <v>3295</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D18" s="8">
         <f>table1_calc!C10</f>
         <v>0.1133998269045961</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <f>table1_calc!E10</f>
         <v>851</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F18" s="8">
         <f>table1_calc!F10</f>
         <v>0.33446088309818073</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <f>table1_calc!G10</f>
         <v>1527</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H18" s="8">
         <f>table1_calc!H10</f>
         <v>0.18993898200570411</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B18" t="str">
+    <row r="19" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B19" t="str">
         <f>table1_calc!D11</f>
         <v>Non-Hispanic White</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <f>table1_calc!B11</f>
         <v>7779</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D19" s="8">
         <f>table1_calc!C11</f>
         <v>0.69979050263761855</v>
       </c>
-      <c r="E18">
+      <c r="E19">
         <f>table1_calc!E11</f>
         <v>987</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F19" s="8">
         <f>table1_calc!F11</f>
         <v>0.12363546706212772</v>
       </c>
-      <c r="G18">
+      <c r="G19">
         <f>table1_calc!G11</f>
         <v>3817</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H19" s="8">
         <f>table1_calc!H11</f>
         <v>2.699818511913054E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B19" t="str">
+    <row r="20" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B20" t="str">
         <f>table1_calc!D12</f>
         <v>Other Hispanic</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <f>table1_calc!B12</f>
         <v>1371</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D20" s="8">
         <f>table1_calc!C12</f>
         <v>4.4311190171690093E-2</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <f>table1_calc!E12</f>
         <v>246</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F20" s="8">
         <f>table1_calc!F12</f>
         <v>1.3878321047044873</v>
       </c>
-      <c r="G19">
+      <c r="G20">
         <f>table1_calc!G12</f>
         <v>519</v>
       </c>
-      <c r="H19" s="8">
+      <c r="H20" s="8">
         <f>table1_calc!H12</f>
         <v>0.54130305462876205</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B20" t="str">
+    <row r="21" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B21" t="str">
         <f>table1_calc!D13</f>
         <v>Other Race - Including Multi-Racial</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <f>table1_calc!B13</f>
         <v>732</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D21" s="8">
         <f>table1_calc!C13</f>
         <v>6.1097425678983346E-2</v>
       </c>
-      <c r="E20">
+      <c r="E21">
         <f>table1_calc!E13</f>
         <v>132</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F21" s="8">
         <f>table1_calc!F13</f>
         <v>0.98342588947265941</v>
       </c>
-      <c r="G20">
+      <c r="G21">
         <f>table1_calc!G13</f>
         <v>293</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H21" s="8">
         <f>table1_calc!H13</f>
         <v>0.36563496248657407</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+    <row r="22" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B22" t="str">
+    <row r="23" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B23" t="str">
         <f>table1_calc!D14</f>
         <v>Missing</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <f>table1_calc!B14</f>
         <v>1004</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D23" s="8">
         <f>table1_calc!C14</f>
         <v>5.7478270001196485E-2</v>
       </c>
-      <c r="E22">
+      <c r="E23">
         <f>table1_calc!E14</f>
         <v>192</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F23" s="8">
         <f>table1_calc!F14</f>
         <v>1.0407092205182975</v>
       </c>
-      <c r="G22">
+      <c r="G23">
         <f>table1_calc!G14</f>
         <v>389</v>
       </c>
-      <c r="H22" s="8">
+      <c r="H23" s="8">
         <f>table1_calc!H14</f>
         <v>0.40853161778256469</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B23" t="str">
+    <row r="24" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B24" t="str">
         <f>table1_calc!D15</f>
         <v>N/A (Male)</v>
       </c>
-      <c r="C23">
+      <c r="C24">
         <f>table1_calc!B15</f>
         <v>7999</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D24" s="8">
         <f>table1_calc!C15</f>
         <v>0.48823728793649102</v>
       </c>
-      <c r="E23">
+      <c r="E24">
         <f>table1_calc!E15</f>
         <v>1296</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F24" s="8">
         <f>table1_calc!F15</f>
         <v>0.14555300154929787</v>
       </c>
-      <c r="G23">
+      <c r="G24">
         <f>table1_calc!G15</f>
         <v>3482</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H24" s="8">
         <f>table1_calc!H15</f>
         <v>4.2651344716308E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B24" t="str">
+    <row r="25" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B25" t="str">
         <f>table1_calc!D16</f>
         <v>No</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <f>table1_calc!B16</f>
         <v>6545</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D25" s="8">
         <f>table1_calc!C16</f>
         <v>0.41109090558527345</v>
       </c>
-      <c r="E24">
+      <c r="E25">
         <f>table1_calc!E16</f>
         <v>1037</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F25" s="8">
         <f>table1_calc!F16</f>
         <v>0.18136941785547411</v>
       </c>
-      <c r="G24">
+      <c r="G25">
         <f>table1_calc!G16</f>
         <v>3188</v>
       </c>
-      <c r="H24" s="8">
+      <c r="H25" s="8">
         <f>table1_calc!H16</f>
         <v>4.5845925676703911E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B25" t="str">
+    <row r="26" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B26" t="str">
         <f>table1_calc!D17</f>
         <v>Yes</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <f>table1_calc!B17</f>
         <v>524</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D26" s="8">
         <f>table1_calc!C17</f>
         <v>4.3193536477039947E-2</v>
       </c>
-      <c r="E25">
+      <c r="E26">
         <f>table1_calc!E17</f>
         <v>68</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F26" s="8">
         <f>table1_calc!F17</f>
         <v>2.1848944842807558</v>
       </c>
-      <c r="G25">
+      <c r="G26">
         <f>table1_calc!G17</f>
         <v>263</v>
       </c>
-      <c r="H25" s="8">
+      <c r="H26" s="8">
         <f>table1_calc!H17</f>
         <v>0.39354558844858495</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="27" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B27" t="str">
+    <row r="28" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B28" t="str">
         <f>table1_calc!D18</f>
         <v>3+ ng/mL</v>
       </c>
-      <c r="C27">
+      <c r="C28">
         <f>table1_calc!B18</f>
         <v>4191</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D28" s="8">
         <f>table1_calc!C18</f>
         <v>0.2668761193923872</v>
       </c>
-      <c r="E27">
+      <c r="E28">
         <f>table1_calc!E18</f>
         <v>840</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F28" s="8">
         <f>table1_calc!F18</f>
         <v>0.20083704085559473</v>
       </c>
-      <c r="G27">
+      <c r="G28">
         <f>table1_calc!G18</f>
         <v>2022</v>
       </c>
-      <c r="H27" s="8">
+      <c r="H28" s="8">
         <f>table1_calc!H18</f>
         <v>7.0698430377132526E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B28" t="str">
+    <row r="29" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B29" t="str">
         <f>table1_calc!D19</f>
         <v>&lt;3 ng/mL</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <f>table1_calc!B19</f>
         <v>11881</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D29" s="8">
         <f>table1_calc!C19</f>
         <v>0.73312388060761347</v>
       </c>
-      <c r="E28">
+      <c r="E29">
         <f>table1_calc!E19</f>
         <v>1753</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F29" s="8">
         <f>table1_calc!F19</f>
         <v>0.11333540321422844</v>
       </c>
-      <c r="G28">
+      <c r="G29">
         <f>table1_calc!G19</f>
         <v>5300</v>
       </c>
-      <c r="H28" s="8">
+      <c r="H29" s="8">
         <f>table1_calc!H19</f>
         <v>2.7699054178133495E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    <row r="30" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B30" t="str">
+    <row r="31" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B31" t="str">
         <f>table1_calc!D20</f>
         <v>Missing</v>
       </c>
-      <c r="C30">
+      <c r="C31">
         <f>table1_calc!B20</f>
         <v>1191</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D31" s="8">
         <f>table1_calc!C20</f>
         <v>7.1414271567199955E-2</v>
       </c>
-      <c r="E30">
+      <c r="E31">
         <f>table1_calc!E20</f>
         <v>212</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F31" s="8">
         <f>table1_calc!F20</f>
         <v>0.88522980032501219</v>
       </c>
-      <c r="G30">
+      <c r="G31">
         <f>table1_calc!G20</f>
         <v>486</v>
       </c>
-      <c r="H30" s="8">
+      <c r="H31" s="8">
         <f>table1_calc!H20</f>
         <v>0.3088644192904253</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B31" t="str">
+    <row r="32" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B32" t="str">
         <f>table1_calc!D21</f>
         <v>N/A (Male)</v>
       </c>
-      <c r="C31">
+      <c r="C32">
         <f>table1_calc!B21</f>
         <v>7999</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D32" s="8">
         <f>table1_calc!C21</f>
         <v>0.48823728793649113</v>
       </c>
-      <c r="E31">
+      <c r="E32">
         <f>table1_calc!E21</f>
         <v>1296</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F32" s="8">
         <f>table1_calc!F21</f>
         <v>0.14555300154929787</v>
       </c>
-      <c r="G31">
+      <c r="G32">
         <f>table1_calc!G21</f>
         <v>3482</v>
       </c>
-      <c r="H31" s="8">
+      <c r="H32" s="8">
         <f>table1_calc!H21</f>
         <v>4.2651344716308E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B32" t="str">
+    <row r="33" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B33" t="str">
         <f>table1_calc!D22</f>
         <v>No</v>
       </c>
-      <c r="C32">
+      <c r="C33">
         <f>table1_calc!B22</f>
         <v>6616</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D33" s="8">
         <f>table1_calc!C22</f>
         <v>0.41965335651746505</v>
       </c>
-      <c r="E32">
+      <c r="E33">
         <f>table1_calc!E22</f>
         <v>1053</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F33" s="8">
         <f>table1_calc!F22</f>
         <v>0.17820433721689671</v>
       </c>
-      <c r="G32">
+      <c r="G33">
         <f>table1_calc!G22</f>
         <v>3190</v>
       </c>
-      <c r="H32" s="8">
+      <c r="H33" s="8">
         <f>table1_calc!H22</f>
         <v>4.5028947847968126E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B33" t="str">
+    <row r="34" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B34" t="str">
         <f>table1_calc!D23</f>
         <v>Yes</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <f>table1_calc!B23</f>
         <v>266</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D34" s="8">
         <f>table1_calc!C23</f>
         <v>2.0695083978845289E-2</v>
       </c>
-      <c r="E33">
+      <c r="E34">
         <f>table1_calc!E23</f>
         <v>32</v>
       </c>
-      <c r="F33" s="8">
+      <c r="F34" s="8">
         <f>table1_calc!F23</f>
         <v>5.2357659140491188</v>
       </c>
-      <c r="G33">
+      <c r="G34">
         <f>table1_calc!G23</f>
         <v>164</v>
       </c>
-      <c r="H33" s="8">
+      <c r="H34" s="8">
         <f>table1_calc!H23</f>
         <v>0.73780101647091811</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="35" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B35" t="str">
+    <row r="36" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B36" t="str">
         <f>table1_calc!D24</f>
         <v>No</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <f>table1_calc!B24</f>
         <v>10262</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D36" s="8">
         <f>table1_calc!C24</f>
         <v>0.65871127222261139</v>
       </c>
-      <c r="E35">
+      <c r="E36">
         <f>table1_calc!E24</f>
         <v>1499</v>
       </c>
-      <c r="F35" s="8">
+      <c r="F36" s="8">
         <f>table1_calc!F24</f>
         <v>0.12031148178383044</v>
       </c>
-      <c r="G35">
+      <c r="G36">
         <f>table1_calc!G24</f>
         <v>4702</v>
       </c>
-      <c r="H35" s="8">
+      <c r="H36" s="8">
         <f>table1_calc!H24</f>
         <v>2.9928217895383562E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B36" t="str">
+    <row r="37" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B37" t="str">
         <f>table1_calc!D25</f>
         <v>Yes</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <f>table1_calc!B25</f>
         <v>5810</v>
       </c>
-      <c r="D36" s="8">
+      <c r="D37" s="8">
         <f>table1_calc!C25</f>
         <v>0.34128872777738872</v>
       </c>
-      <c r="E36">
+      <c r="E37">
         <f>table1_calc!E25</f>
         <v>1094</v>
       </c>
-      <c r="F36" s="8">
+      <c r="F37" s="8">
         <f>table1_calc!F25</f>
         <v>0.18212379205832899</v>
       </c>
-      <c r="G36">
+      <c r="G37">
         <f>table1_calc!G25</f>
         <v>2620</v>
       </c>
-      <c r="H36" s="8">
+      <c r="H37" s="8">
         <f>table1_calc!H25</f>
         <v>5.9404933093248555E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="38" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B38" t="str">
+    <row r="39" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B39" t="str">
         <f>table1_calc!D26</f>
         <v>Missing</v>
       </c>
-      <c r="C38">
+      <c r="C39">
         <f>table1_calc!B26</f>
         <v>4442</v>
       </c>
-      <c r="D38" s="8">
+      <c r="D39" s="8">
         <f>table1_calc!C26</f>
         <v>0.32367441707480754</v>
       </c>
-      <c r="E38">
+      <c r="E39">
         <f>table1_calc!E26</f>
         <v>695</v>
       </c>
-      <c r="F38" s="8">
+      <c r="F39" s="8">
         <f>table1_calc!F26</f>
         <v>0.22935218210166777</v>
       </c>
-      <c r="G38">
+      <c r="G39">
         <f>table1_calc!G26</f>
         <v>3270</v>
       </c>
-      <c r="H38" s="8">
+      <c r="H39" s="8">
         <f>table1_calc!H26</f>
         <v>4.015740887290007E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B39" t="str">
+    <row r="40" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B40" t="str">
         <f>table1_calc!D27</f>
         <v>No</v>
       </c>
-      <c r="C39">
+      <c r="C40">
         <f>table1_calc!B27</f>
         <v>3409</v>
       </c>
-      <c r="D39" s="8">
+      <c r="D40" s="8">
         <f>table1_calc!C27</f>
         <v>0.15919464430513561</v>
       </c>
-      <c r="E39">
+      <c r="E40">
         <f>table1_calc!E27</f>
         <v>594</v>
       </c>
-      <c r="F39" s="8">
+      <c r="F40" s="8">
         <f>table1_calc!F27</f>
         <v>0.40682157851254425</v>
       </c>
-      <c r="G39">
+      <c r="G40">
         <f>table1_calc!G27</f>
         <v>1188</v>
       </c>
-      <c r="H39" s="8">
+      <c r="H40" s="8">
         <f>table1_calc!H27</f>
         <v>0.17506449514044789</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B40" t="str">
+    <row r="41" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B41" t="str">
         <f>table1_calc!D28</f>
         <v>Yes</v>
       </c>
-      <c r="C40">
+      <c r="C41">
         <f>table1_calc!B28</f>
         <v>8221</v>
       </c>
-      <c r="D40" s="8">
+      <c r="D41" s="8">
         <f>table1_calc!C28</f>
         <v>0.51713093862005621</v>
       </c>
-      <c r="E40">
+      <c r="E41">
         <f>table1_calc!E28</f>
         <v>1304</v>
       </c>
-      <c r="F40" s="8">
+      <c r="F41" s="8">
         <f>table1_calc!F28</f>
         <v>0.14317739671505431</v>
       </c>
-      <c r="G40">
+      <c r="G41">
         <f>table1_calc!G28</f>
         <v>2864</v>
       </c>
-      <c r="H40" s="8">
+      <c r="H41" s="8">
         <f>table1_calc!H28</f>
         <v>5.0935388328345002E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+    <row r="42" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B42" t="str">
+    <row r="43" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B43" t="str">
         <f>table1_calc!D29</f>
         <v>0-100%</v>
       </c>
-      <c r="C42">
+      <c r="C43">
         <f>table1_calc!B29</f>
         <v>4316</v>
       </c>
-      <c r="D42" s="8">
+      <c r="D43" s="8">
         <f>table1_calc!C29</f>
         <v>0.18972914844892752</v>
       </c>
-      <c r="E42">
+      <c r="E43">
         <f>table1_calc!E29</f>
         <v>839</v>
       </c>
-      <c r="F42" s="8">
+      <c r="F43" s="8">
         <f>table1_calc!F29</f>
         <v>0.28186311462383357</v>
       </c>
-      <c r="G42">
+      <c r="G43">
         <f>table1_calc!G29</f>
         <v>1778</v>
       </c>
-      <c r="H42" s="8">
+      <c r="H43" s="8">
         <f>table1_calc!H29</f>
         <v>0.1158921091444377</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B43" t="str">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B44" t="str">
         <f>table1_calc!D30</f>
         <v>100-199%</v>
       </c>
-      <c r="C43">
+      <c r="C44">
         <f>table1_calc!B30</f>
         <v>3962</v>
       </c>
-      <c r="D43" s="8">
+      <c r="D44" s="8">
         <f>table1_calc!C30</f>
         <v>0.18997926591229689</v>
       </c>
-      <c r="E43">
+      <c r="E44">
         <f>table1_calc!E30</f>
         <v>683</v>
       </c>
-      <c r="F43" s="8">
+      <c r="F44" s="8">
         <f>table1_calc!F30</f>
         <v>0.31149436051360679</v>
       </c>
-      <c r="G43">
+      <c r="G44">
         <f>table1_calc!G30</f>
         <v>1794</v>
       </c>
-      <c r="H43" s="8">
+      <c r="H44" s="8">
         <f>table1_calc!H30</f>
         <v>0.1037529368190445</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B44" t="str">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45" t="str">
         <f>table1_calc!D31</f>
         <v>200%+</v>
       </c>
-      <c r="C44">
+      <c r="C45">
         <f>table1_calc!B31</f>
         <v>7794</v>
       </c>
-      <c r="D44" s="8">
+      <c r="D45" s="8">
         <f>table1_calc!C31</f>
         <v>0.62029158563877485</v>
       </c>
-      <c r="E44">
+      <c r="E45">
         <f>table1_calc!E31</f>
         <v>1071</v>
       </c>
-      <c r="F44" s="8">
+      <c r="F45" s="8">
         <f>table1_calc!F31</f>
         <v>0.14195719450661229</v>
       </c>
-      <c r="G44">
+      <c r="G45">
         <f>table1_calc!G31</f>
         <v>3750</v>
       </c>
-      <c r="H44" s="8">
+      <c r="H45" s="8">
         <f>table1_calc!H31</f>
         <v>3.1269636557201927E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B46" t="str">
-        <f>table1_calc!D32</f>
-        <v>No</v>
-      </c>
-      <c r="C46">
-        <f>table1_calc!B32</f>
-        <v>8741</v>
-      </c>
-      <c r="D46" s="8">
-        <f>table1_calc!C32</f>
-        <v>0.49753098650550065</v>
-      </c>
-      <c r="E46">
-        <f>table1_calc!E32</f>
-        <v>1143</v>
-      </c>
-      <c r="F46" s="8">
-        <f>table1_calc!F32</f>
-        <v>0.18571772250622728</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B47" t="str">
-        <f>table1_calc!D33</f>
-        <v>Yes</v>
-      </c>
-      <c r="C47">
-        <f>table1_calc!B33</f>
-        <v>7322</v>
-      </c>
-      <c r="D47" s="8">
-        <f>table1_calc!C33</f>
-        <v>0.50246901349449935</v>
-      </c>
-      <c r="E47">
-        <f>table1_calc!E33</f>
-        <v>1448</v>
-      </c>
-      <c r="F47" s="8">
-        <f>table1_calc!F33</f>
-        <v>0.1189148184844568</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B49" t="str">
-        <f>table1_calc!D34</f>
-        <v>No</v>
-      </c>
-      <c r="C49">
-        <f>table1_calc!B34</f>
-        <v>13460</v>
-      </c>
-      <c r="D49" s="8">
-        <f>table1_calc!C34</f>
-        <v>0.86197470541915644</v>
-      </c>
-      <c r="G49">
-        <f>table1_calc!G34</f>
-        <v>5862</v>
-      </c>
-      <c r="H49" s="8">
-        <f>table1_calc!H34</f>
-        <v>2.3909812280776207E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B50" t="str">
-        <f>table1_calc!D35</f>
-        <v>Yes</v>
-      </c>
-      <c r="C50">
-        <f>table1_calc!B35</f>
-        <v>2593</v>
-      </c>
-      <c r="D50" s="8">
-        <f>table1_calc!C35</f>
-        <v>0.13802529458084356</v>
-      </c>
-      <c r="G50">
-        <f>table1_calc!G35</f>
-        <v>1448</v>
-      </c>
-      <c r="H50" s="8">
-        <f>table1_calc!H35</f>
-        <v>0.1189148184844568</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B52" t="str">
         <f>table1_calc!D36</f>
         <v>Missing</v>
       </c>
-      <c r="C52">
+      <c r="C47">
         <f>table1_calc!B36</f>
         <v>612</v>
       </c>
-      <c r="D52" s="8">
+      <c r="D47" s="8">
         <f>table1_calc!C36</f>
         <v>4.0553480625368683E-2</v>
       </c>
-      <c r="E52">
+      <c r="E47">
         <f>table1_calc!E36</f>
         <v>153</v>
       </c>
-      <c r="F52" s="8">
+      <c r="F47" s="8">
         <f>table1_calc!F36</f>
         <v>1.1499444556588043</v>
       </c>
-      <c r="G52">
+      <c r="G47">
         <f>table1_calc!G36</f>
         <v>548</v>
       </c>
-      <c r="H52" s="8">
+      <c r="H47" s="8">
         <f>table1_calc!H36</f>
         <v>0.27267546982870033</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B53" t="str">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B48" t="str">
         <f>table1_calc!D37</f>
         <v>No</v>
       </c>
-      <c r="C53">
+      <c r="C48">
         <f>table1_calc!B37</f>
         <v>14659</v>
       </c>
-      <c r="D53" s="8">
+      <c r="D48" s="8">
         <f>table1_calc!C37</f>
         <v>0.90202366472776174</v>
       </c>
-      <c r="E53">
+      <c r="E48">
         <f>table1_calc!E37</f>
         <v>2246</v>
       </c>
-      <c r="F53" s="8">
+      <c r="F48" s="8">
         <f>table1_calc!F37</f>
         <v>8.5412835496502942E-2</v>
       </c>
-      <c r="G53">
+      <c r="G48">
         <f>table1_calc!G37</f>
         <v>6013</v>
       </c>
-      <c r="H53" s="8">
+      <c r="H48" s="8">
         <f>table1_calc!H37</f>
         <v>2.4353134544644169E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B54" t="str">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" t="str">
         <f>table1_calc!D38</f>
         <v>Yes</v>
       </c>
-      <c r="C54">
+      <c r="C49">
         <f>table1_calc!B38</f>
         <v>801</v>
       </c>
-      <c r="D54" s="8">
+      <c r="D49" s="8">
         <f>table1_calc!C38</f>
         <v>5.7422854646869054E-2</v>
       </c>
-      <c r="E54">
+      <c r="E49">
         <f>table1_calc!E38</f>
         <v>194</v>
       </c>
-      <c r="F54" s="8">
+      <c r="F49" s="8">
         <f>table1_calc!F38</f>
         <v>0.81627319806786525</v>
       </c>
-      <c r="G54">
+      <c r="G49">
         <f>table1_calc!G38</f>
         <v>761</v>
       </c>
-      <c r="H54" s="8">
+      <c r="H49" s="8">
         <f>table1_calc!H38</f>
         <v>0.18125588642003937</v>
       </c>
@@ -2315,8 +2255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3297,7 +3237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -3310,7 +3250,7 @@
   <sheetData>
     <row r="1" spans="1:8" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -3321,21 +3261,21 @@
       <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A3" s="15"/>
       <c r="B3" s="15"/>
       <c r="C3" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
@@ -3449,7 +3389,7 @@
     </row>
     <row r="14" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="3" t="str">
@@ -3579,7 +3519,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="3" t="str">
@@ -3719,7 +3659,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="3" t="str">
@@ -3769,7 +3709,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="3" t="str">
@@ -3849,7 +3789,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="3" t="str">
@@ -3879,7 +3819,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="3" t="str">
@@ -3909,7 +3849,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="3" t="str">
@@ -3939,7 +3879,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="3" t="str">
@@ -4003,16 +3943,16 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" t="s">
         <v>85</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>86</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>87</v>
-      </c>
-      <c r="D1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4020,13 +3960,13 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C2">
         <v>0.44000978672709373</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E2" t="str">
         <f>SUBSTITUTE(B2,A2&amp;" ","")</f>
@@ -4044,7 +3984,7 @@
         <v>0.3096591365990401</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E51" si="0">SUBSTITUTE(B3,A3&amp;" ","")</f>
@@ -4062,7 +4002,7 @@
         <v>0.41303603557316559</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
@@ -4080,7 +4020,7 @@
         <v>0.43793037794309775</v>
       </c>
       <c r="D5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
@@ -4098,7 +4038,7 @@
         <v>0.39242336486993951</v>
       </c>
       <c r="D6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
@@ -4116,7 +4056,7 @@
         <v>0.4478844288564599</v>
       </c>
       <c r="D7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
@@ -4134,7 +4074,7 @@
         <v>0.4090881543949349</v>
       </c>
       <c r="D8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
@@ -4152,7 +4092,7 @@
         <v>0.35851010276317385</v>
       </c>
       <c r="D9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
@@ -4164,13 +4104,13 @@
         <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10">
         <v>0.40547504092767822</v>
       </c>
       <c r="D10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
@@ -4182,13 +4122,13 @@
         <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C11">
         <v>0.49476133241707776</v>
       </c>
       <c r="D11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
@@ -4200,13 +4140,13 @@
         <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C12">
         <v>0.33842027476555847</v>
       </c>
       <c r="D12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
@@ -4218,13 +4158,13 @@
         <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C13">
         <v>0.44160891208178438</v>
       </c>
       <c r="D13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
@@ -4236,13 +4176,13 @@
         <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C14">
         <v>0.32483172576271202</v>
       </c>
       <c r="D14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
@@ -4254,13 +4194,13 @@
         <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C15">
         <v>0.40157495210669342</v>
       </c>
       <c r="D15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
@@ -4272,13 +4212,13 @@
         <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C16">
         <v>0.49906557112167471</v>
       </c>
       <c r="D16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
@@ -4290,13 +4230,13 @@
         <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C17">
         <v>0.37717799598252866</v>
       </c>
       <c r="D17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
@@ -4308,13 +4248,13 @@
         <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C18">
         <v>0.3841963615684636</v>
       </c>
       <c r="D18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
@@ -4326,13 +4266,13 @@
         <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C19">
         <v>0.24603710160028339</v>
       </c>
       <c r="D19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
@@ -4341,16 +4281,16 @@
     </row>
     <row r="20" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" t="s">
         <v>101</v>
-      </c>
-      <c r="B20" t="s">
-        <v>102</v>
       </c>
       <c r="C20">
         <v>0.31214897785156609</v>
       </c>
       <c r="D20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="0"/>
@@ -4359,16 +4299,16 @@
     </row>
     <row r="21" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C21">
         <v>0.35326602039781346</v>
       </c>
       <c r="D21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
@@ -4377,16 +4317,16 @@
     </row>
     <row r="22" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C22">
         <v>0.33051079085146839</v>
       </c>
       <c r="D22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="0"/>
@@ -4395,16 +4335,16 @@
     </row>
     <row r="23" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C23">
         <v>0.33816145174012491</v>
       </c>
       <c r="D23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
@@ -4413,16 +4353,16 @@
     </row>
     <row r="24" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C24">
         <v>0.37110867368389777</v>
       </c>
       <c r="D24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
@@ -4431,16 +4371,16 @@
     </row>
     <row r="25" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C25">
         <v>0.41304323205675048</v>
       </c>
       <c r="D25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
@@ -4449,16 +4389,16 @@
     </row>
     <row r="26" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C26">
         <v>0.39089648983562331</v>
       </c>
       <c r="D26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="0"/>
@@ -4467,16 +4407,16 @@
     </row>
     <row r="27" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C27">
         <v>0.37146265494871394</v>
       </c>
       <c r="D27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="0"/>
@@ -4485,16 +4425,16 @@
     </row>
     <row r="28" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C28">
         <v>0.45205734989945134</v>
       </c>
       <c r="D28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="0"/>
@@ -4503,16 +4443,16 @@
     </row>
     <row r="29" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C29">
         <v>0.45511898391270111</v>
       </c>
       <c r="D29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="0"/>
@@ -4521,16 +4461,16 @@
     </row>
     <row r="30" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C30">
         <v>0.46615149843047488</v>
       </c>
       <c r="D30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="0"/>
@@ -4539,16 +4479,16 @@
     </row>
     <row r="31" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C31">
         <v>0.4308811088606016</v>
       </c>
       <c r="D31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="0"/>
@@ -4557,16 +4497,16 @@
     </row>
     <row r="32" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C32">
         <v>0.46646622557116207</v>
       </c>
       <c r="D32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="0"/>
@@ -4578,13 +4518,13 @@
         <v>51</v>
       </c>
       <c r="B33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C33">
         <v>0.42473342829893801</v>
       </c>
       <c r="D33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="0"/>
@@ -4596,13 +4536,13 @@
         <v>51</v>
       </c>
       <c r="B34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C34">
         <v>0.32483172576271202</v>
       </c>
       <c r="D34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" si="0"/>
@@ -4614,13 +4554,13 @@
         <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C35">
         <v>0.42950354584615968</v>
       </c>
       <c r="D35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E35" t="str">
         <f t="shared" si="0"/>
@@ -4632,13 +4572,13 @@
         <v>51</v>
       </c>
       <c r="B36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C36">
         <v>0.57458942602835883</v>
       </c>
       <c r="D36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" si="0"/>
@@ -4650,13 +4590,13 @@
         <v>56</v>
       </c>
       <c r="B37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C37">
         <v>0.4032064044457197</v>
       </c>
       <c r="D37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E37" t="str">
         <f t="shared" si="0"/>
@@ -4668,13 +4608,13 @@
         <v>56</v>
       </c>
       <c r="B38" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C38">
         <v>0.37729194839251184</v>
       </c>
       <c r="D38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E38" t="str">
         <f t="shared" si="0"/>
@@ -4686,13 +4626,13 @@
         <v>59</v>
       </c>
       <c r="B39" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C39">
         <v>0.41676188862562952</v>
       </c>
       <c r="D39" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E39" t="str">
         <f t="shared" si="0"/>
@@ -4704,13 +4644,13 @@
         <v>59</v>
       </c>
       <c r="B40" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C40">
         <v>0.32483172576271202</v>
       </c>
       <c r="D40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" si="0"/>
@@ -4722,13 +4662,13 @@
         <v>59</v>
       </c>
       <c r="B41" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C41">
         <v>0.43646158511522049</v>
       </c>
       <c r="D41" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E41" t="str">
         <f t="shared" si="0"/>
@@ -4740,13 +4680,13 @@
         <v>59</v>
       </c>
       <c r="B42" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C42">
         <v>0.61713639461731518</v>
       </c>
       <c r="D42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E42" t="str">
         <f t="shared" si="0"/>
@@ -4758,13 +4698,13 @@
         <v>60</v>
       </c>
       <c r="B43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C43">
         <v>0.2795317042568769</v>
       </c>
       <c r="D43" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E43" t="str">
         <f t="shared" si="0"/>
@@ -4776,13 +4716,13 @@
         <v>60</v>
       </c>
       <c r="B44" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C44">
         <v>0.58683407580468716</v>
       </c>
       <c r="D44" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E44" t="str">
         <f t="shared" si="0"/>
@@ -4794,13 +4734,13 @@
         <v>63</v>
       </c>
       <c r="B45" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C45">
         <v>0.37007476165686526</v>
       </c>
       <c r="D45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E45" t="str">
         <f t="shared" si="0"/>
@@ -4812,13 +4752,13 @@
         <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C46">
         <v>0.39893239189163154</v>
       </c>
       <c r="D46" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E46" t="str">
         <f t="shared" si="0"/>
@@ -4830,13 +4770,13 @@
         <v>64</v>
       </c>
       <c r="B47" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C47">
         <v>0.37430583548502194</v>
       </c>
       <c r="D47" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E47" t="str">
         <f t="shared" si="0"/>
@@ -4848,13 +4788,13 @@
         <v>64</v>
       </c>
       <c r="B48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C48">
         <v>0.4489461786678155</v>
       </c>
       <c r="D48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E48" t="str">
         <f t="shared" si="0"/>
@@ -4866,13 +4806,13 @@
         <v>65</v>
       </c>
       <c r="B49" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C49">
         <v>0.51068268876384093</v>
       </c>
       <c r="D49" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E49" t="str">
         <f t="shared" si="0"/>
@@ -4884,13 +4824,13 @@
         <v>65</v>
       </c>
       <c r="B50" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C50">
         <v>0.37574689101038272</v>
       </c>
       <c r="D50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E50" t="str">
         <f t="shared" si="0"/>
@@ -4902,13 +4842,13 @@
         <v>65</v>
       </c>
       <c r="B51" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C51">
         <v>0.43419790414009329</v>
       </c>
       <c r="D51" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E51" t="str">
         <f t="shared" si="0"/>
@@ -4924,8 +4864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4942,64 +4882,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+    </row>
+    <row r="2" spans="1:10" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="27" t="s">
         <v>153</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-    </row>
-    <row r="2" spans="1:10" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="24" t="s">
-        <v>154</v>
-      </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27" t="s">
-        <v>162</v>
-      </c>
-      <c r="J3" s="27"/>
+      <c r="J3" s="30"/>
     </row>
     <row r="4" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>0</v>
@@ -5007,7 +4947,7 @@
     </row>
     <row r="5" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
@@ -5092,30 +5032,30 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E8" s="2">
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="G8" s="28" t="s">
-        <v>165</v>
+        <v>164</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>164</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="I8" s="28" t="s">
-        <v>165</v>
+        <v>164</v>
+      </c>
+      <c r="I8" s="22" t="s">
+        <v>164</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -5243,19 +5183,19 @@
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E14" s="6">
         <v>1</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>165</v>
+        <v>164</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>164</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -5271,22 +5211,22 @@
       <c r="J15" s="7"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
+      <c r="A16" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -5347,13 +5287,13 @@
         <v>19</v>
       </c>
       <c r="K1" t="s">
+        <v>157</v>
+      </c>
+      <c r="L1" t="s">
         <v>158</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>159</v>
-      </c>
-      <c r="M1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added supplemental table 1
</commit_message>
<xml_diff>
--- a/final_tables_4.24.17.xlsx
+++ b/final_tables_4.24.17.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Audrey\Documents\nhanes_ses_sleep_crp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7305" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="4" r:id="rId1"/>
@@ -13,8 +18,10 @@
     <sheet name="table2_calc" sheetId="6" r:id="rId4"/>
     <sheet name="Table 3" sheetId="1" r:id="rId5"/>
     <sheet name="table3_calc" sheetId="2" r:id="rId6"/>
+    <sheet name="Supplementary Table 1" sheetId="7" r:id="rId7"/>
+    <sheet name="suppl_tbl1_calc" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="164">
   <si>
     <t>95% CI</t>
   </si>
@@ -537,23 +544,125 @@
     <t>Geometric mean CRP (mg/L)</t>
   </si>
   <si>
-    <t>P-value (ANOVA*)</t>
-  </si>
-  <si>
     <t>*ANOVA models fit using CRP transformed by the natural logarithm.</t>
   </si>
   <si>
     <t>Table 2. Geometric mean plasma c-reactive protein (CRP).</t>
+  </si>
+  <si>
+    <t>ss_x2</t>
+  </si>
+  <si>
+    <t>ss_df</t>
+  </si>
+  <si>
+    <t>ss_p</t>
+  </si>
+  <si>
+    <t>ps_x2</t>
+  </si>
+  <si>
+    <t>ps_df</t>
+  </si>
+  <si>
+    <t>ps_p</t>
+  </si>
+  <si>
+    <t>crp</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>C-reactive protein</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>DF</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>P-value*</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Supplementary table 1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Results of examining whether each hypothesized mediator was associated with each exposure and the outcome. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Χ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>*Values are F statistic, rather than X</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="175" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -589,6 +698,42 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -639,7 +784,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -698,6 +843,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -719,16 +874,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="175" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1002,7 +1177,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1012,46 +1187,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="32.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="8" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="2.08984375" customWidth="1"/>
+    <col min="2" max="2" width="13.08984375" customWidth="1"/>
+    <col min="3" max="3" width="7.26953125" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="6.26953125" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="5.90625" customWidth="1"/>
+    <col min="8" max="8" width="10.54296875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-    </row>
-    <row r="2" spans="1:9" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="26" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26" t="s">
+      <c r="D2" s="30"/>
+      <c r="E2" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26" t="s">
+      <c r="F2" s="30"/>
+      <c r="G2" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="26"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H2" s="30"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>82</v>
       </c>
@@ -1078,7 +1256,7 @@
       </c>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="24" t="s">
         <v>138</v>
       </c>
@@ -1107,7 +1285,7 @@
       </c>
       <c r="I4" s="12"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>118</v>
       </c>
@@ -1130,7 +1308,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>121</v>
       </c>
@@ -1153,7 +1331,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1164,7 +1342,7 @@
       <c r="G7" s="5"/>
       <c r="H7" s="9"/>
     </row>
-    <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B8" t="str">
         <f>table1_calc!D2</f>
         <v>9-11th Grade (Includes 12th grade with no diploma)</v>
@@ -1194,7 +1372,7 @@
         <v>0.16353579652259004</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" t="str">
         <f>table1_calc!D3</f>
         <v>College Graduate or above</v>
@@ -1224,7 +1402,7 @@
         <v>7.692342920565258E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" t="str">
         <f>table1_calc!D4</f>
         <v>High School Grad/GED or Equivalent</v>
@@ -1254,7 +1432,7 @@
         <v>7.7853288514700261E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" t="str">
         <f>table1_calc!D5</f>
         <v>Less Than 9th Grade</v>
@@ -1284,7 +1462,7 @@
         <v>0.35136132907319062</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" t="str">
         <f>table1_calc!D6</f>
         <v>Some College or AA degree</v>
@@ -1314,12 +1492,12 @@
         <v>6.4637022887462092E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B14" t="str">
         <f>table1_calc!D7</f>
         <v>Female</v>
@@ -1349,7 +1527,7 @@
         <v>3.7312066034715763E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B15" t="str">
         <f>table1_calc!D8</f>
         <v>Male</v>
@@ -1379,12 +1557,12 @@
         <v>4.2651344716308E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B17" t="str">
         <f>table1_calc!D9</f>
         <v>Mexican American</v>
@@ -1414,7 +1592,7 @@
         <v>0.29760454605550918</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B18" t="str">
         <f>table1_calc!D10</f>
         <v>Non-Hispanic Black</v>
@@ -1444,7 +1622,7 @@
         <v>0.18993898200570411</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B19" t="str">
         <f>table1_calc!D11</f>
         <v>Non-Hispanic White</v>
@@ -1474,7 +1652,7 @@
         <v>2.699818511913054E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B20" t="str">
         <f>table1_calc!D12</f>
         <v>Other Hispanic</v>
@@ -1504,7 +1682,7 @@
         <v>0.54130305462876205</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B21" t="str">
         <f>table1_calc!D13</f>
         <v>Other Race - Including Multi-Racial</v>
@@ -1534,12 +1712,12 @@
         <v>0.36563496248657407</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B23" t="str">
         <f>table1_calc!D14</f>
         <v>Missing</v>
@@ -1569,7 +1747,7 @@
         <v>0.40853161778256469</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B24" t="str">
         <f>table1_calc!D15</f>
         <v>N/A (Male)</v>
@@ -1599,7 +1777,7 @@
         <v>4.2651344716308E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B25" t="str">
         <f>table1_calc!D16</f>
         <v>No</v>
@@ -1629,7 +1807,7 @@
         <v>4.5845925676703911E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B26" t="str">
         <f>table1_calc!D17</f>
         <v>Yes</v>
@@ -1659,12 +1837,12 @@
         <v>0.39354558844858495</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B28" t="str">
         <f>table1_calc!D18</f>
         <v>3+ ng/mL</v>
@@ -1694,7 +1872,7 @@
         <v>7.0698430377132526E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B29" t="str">
         <f>table1_calc!D19</f>
         <v>&lt;3 ng/mL</v>
@@ -1724,12 +1902,12 @@
         <v>2.7699054178133495E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B31" t="str">
         <f>table1_calc!D20</f>
         <v>Missing</v>
@@ -1759,7 +1937,7 @@
         <v>0.3088644192904253</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B32" t="str">
         <f>table1_calc!D21</f>
         <v>N/A (Male)</v>
@@ -1789,7 +1967,7 @@
         <v>4.2651344716308E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B33" t="str">
         <f>table1_calc!D22</f>
         <v>No</v>
@@ -1819,7 +1997,7 @@
         <v>4.5028947847968126E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B34" t="str">
         <f>table1_calc!D23</f>
         <v>Yes</v>
@@ -1849,12 +2027,12 @@
         <v>0.73780101647091811</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B36" t="str">
         <f>table1_calc!D24</f>
         <v>No</v>
@@ -1884,7 +2062,7 @@
         <v>2.9928217895383562E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B37" t="str">
         <f>table1_calc!D25</f>
         <v>Yes</v>
@@ -1914,12 +2092,12 @@
         <v>5.9404933093248555E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B39" t="str">
         <f>table1_calc!D26</f>
         <v>Missing</v>
@@ -1949,7 +2127,7 @@
         <v>4.015740887290007E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B40" t="str">
         <f>table1_calc!D27</f>
         <v>No</v>
@@ -1979,7 +2157,7 @@
         <v>0.17506449514044789</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B41" t="str">
         <f>table1_calc!D28</f>
         <v>Yes</v>
@@ -2009,12 +2187,12 @@
         <v>5.0935388328345002E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B43" t="str">
         <f>table1_calc!D29</f>
         <v>0-100%</v>
@@ -2044,7 +2222,7 @@
         <v>0.1158921091444377</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B44" t="str">
         <f>table1_calc!D30</f>
         <v>100-199%</v>
@@ -2074,7 +2252,7 @@
         <v>0.1037529368190445</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B45" t="str">
         <f>table1_calc!D31</f>
         <v>200%+</v>
@@ -2104,12 +2282,12 @@
         <v>3.1269636557201927E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B47" t="str">
         <f>table1_calc!D36</f>
         <v>Missing</v>
@@ -2139,7 +2317,7 @@
         <v>0.27267546982870033</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B48" t="str">
         <f>table1_calc!D37</f>
         <v>No</v>
@@ -2169,32 +2347,33 @@
         <v>2.4353134544644169E-2</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" t="str">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4" t="str">
         <f>table1_calc!D38</f>
         <v>Yes</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="4">
         <f>table1_calc!B38</f>
         <v>801</v>
       </c>
-      <c r="D49" s="8">
+      <c r="D49" s="37">
         <f>table1_calc!C38</f>
         <v>5.7422854646869054E-2</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="4">
         <f>table1_calc!E38</f>
         <v>194</v>
       </c>
-      <c r="F49" s="8">
+      <c r="F49" s="37">
         <f>table1_calc!F38</f>
         <v>0.81627319806786525</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="4">
         <f>table1_calc!G38</f>
         <v>761</v>
       </c>
-      <c r="H49" s="8">
+      <c r="H49" s="37">
         <f>table1_calc!H38</f>
         <v>0.18125588642003937</v>
       </c>
@@ -2218,12 +2397,12 @@
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -2249,7 +2428,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -2275,7 +2454,7 @@
         <v>0.16353579652259004</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -2301,7 +2480,7 @@
         <v>7.692342920565258E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -2327,7 +2506,7 @@
         <v>7.7853288514700261E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -2353,7 +2532,7 @@
         <v>0.35136132907319062</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -2379,7 +2558,7 @@
         <v>6.4637022887462092E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -2405,7 +2584,7 @@
         <v>3.7312066034715763E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -2431,7 +2610,7 @@
         <v>4.2651344716308E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -2457,7 +2636,7 @@
         <v>0.29760454605550918</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -2483,7 +2662,7 @@
         <v>0.18993898200570411</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -2509,7 +2688,7 @@
         <v>2.699818511913054E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -2535,7 +2714,7 @@
         <v>0.54130305462876205</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -2561,7 +2740,7 @@
         <v>0.36563496248657407</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -2587,7 +2766,7 @@
         <v>0.40853161778256469</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -2613,7 +2792,7 @@
         <v>4.2651344716308E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -2639,7 +2818,7 @@
         <v>4.5845925676703911E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -2665,7 +2844,7 @@
         <v>0.39354558844858495</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -2691,7 +2870,7 @@
         <v>7.0698430377132526E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -2717,7 +2896,7 @@
         <v>2.7699054178133495E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -2743,7 +2922,7 @@
         <v>0.3088644192904253</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -2769,7 +2948,7 @@
         <v>4.2651344716308E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -2795,7 +2974,7 @@
         <v>4.5028947847968126E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -2821,7 +3000,7 @@
         <v>0.73780101647091811</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>60</v>
       </c>
@@ -2847,7 +3026,7 @@
         <v>2.9928217895383562E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>60</v>
       </c>
@@ -2873,7 +3052,7 @@
         <v>5.9404933093248555E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -2899,7 +3078,7 @@
         <v>4.015740887290007E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -2925,7 +3104,7 @@
         <v>0.17506449514044789</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -2951,7 +3130,7 @@
         <v>5.0935388328345002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -2977,7 +3156,7 @@
         <v>0.1158921091444377</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>62</v>
       </c>
@@ -3003,7 +3182,7 @@
         <v>0.1037529368190445</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>62</v>
       </c>
@@ -3029,7 +3208,7 @@
         <v>3.1269636557201927E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -3049,7 +3228,7 @@
         <v>0.18571772250622728</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -3069,7 +3248,7 @@
         <v>0.1189148184844568</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -3089,7 +3268,7 @@
         <v>2.3909812280776207E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>64</v>
       </c>
@@ -3109,7 +3288,7 @@
         <v>0.1189148184844568</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -3135,7 +3314,7 @@
         <v>0.27267546982870033</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>65</v>
       </c>
@@ -3161,7 +3340,7 @@
         <v>2.4353134544644169E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>65</v>
       </c>
@@ -3196,20 +3375,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection sqref="A1:D68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="48.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="4.08984375" customWidth="1"/>
+    <col min="2" max="2" width="43.08984375" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -3219,29 +3399,29 @@
       <c r="G1" s="14"/>
       <c r="H1" s="14"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-    </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+    </row>
+    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="15"/>
       <c r="B3" s="15"/>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="D3" s="36" t="s">
-        <v>146</v>
+      <c r="D3" s="29" t="s">
+        <v>160</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
       <c r="G3" s="15"/>
       <c r="H3" s="16"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>138</v>
       </c>
@@ -3253,8 +3433,8 @@
       <c r="G4" s="15"/>
       <c r="H4" s="16"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="24" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="15"/>
@@ -3264,7 +3444,7 @@
         <v>&lt;0.0001</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B6" t="str">
         <f>table2_calc!F2</f>
         <v>9-11th Grade (Includes 12th grade with no diploma)</v>
@@ -3274,7 +3454,7 @@
         <v>0.20597082564191388</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B7" t="str">
         <f>table2_calc!F3</f>
         <v>College Graduate or above</v>
@@ -3284,7 +3464,7 @@
         <v>0.1324012443088248</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B8" t="str">
         <f>table2_calc!F4</f>
         <v>High School Grad/GED or Equivalent</v>
@@ -3294,7 +3474,7 @@
         <v>0.19382391348629144</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B9" t="str">
         <f>table2_calc!F5</f>
         <v>Less Than 9th Grade</v>
@@ -3304,7 +3484,7 @@
         <v>0.2038299658849701</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B10" t="str">
         <f>table2_calc!F6</f>
         <v>Some College or AA degree</v>
@@ -3314,7 +3494,7 @@
         <v>0.17491922473584842</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>79</v>
       </c>
@@ -3323,7 +3503,7 @@
         <v>&lt;0.0001</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B12" t="str">
         <f>table2_calc!F7</f>
         <v>0-100%</v>
@@ -3333,7 +3513,7 @@
         <v>0.19378954272376392</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B13" t="str">
         <f>table2_calc!F8</f>
         <v>100-199%</v>
@@ -3343,7 +3523,7 @@
         <v>0.19351952704729519</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B14" t="str">
         <f>table2_calc!F9</f>
         <v>200%+</v>
@@ -3353,7 +3533,7 @@
         <v>0.15984129219753143</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>109</v>
       </c>
@@ -3362,7 +3542,7 @@
         <v>&lt;0.0001</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B16" t="str">
         <f>table2_calc!F10</f>
         <v>Missing</v>
@@ -3372,7 +3552,7 @@
         <v>0.18428802217283879</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B17" t="str">
         <f>table2_calc!F11</f>
         <v>No</v>
@@ -3382,7 +3562,7 @@
         <v>0.23397085117818919</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B18" t="str">
         <f>table2_calc!F12</f>
         <v>Yes</v>
@@ -3392,7 +3572,7 @@
         <v>0.1497332017604846</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -3401,7 +3581,7 @@
         <v>&lt;0.0001</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B20" t="str">
         <f>table2_calc!F13</f>
         <v>Female</v>
@@ -3411,7 +3591,7 @@
         <v>0.19724557055808828</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B21" t="str">
         <f>table2_calc!F14</f>
         <v>Male</v>
@@ -3421,7 +3601,7 @@
         <v>0.14851840777308084</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>73</v>
       </c>
@@ -3430,7 +3610,7 @@
         <v>&lt;0.0001</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B23" t="str">
         <f>table2_calc!F15</f>
         <v>Mexican American</v>
@@ -3440,7 +3620,7 @@
         <v>0.19827848213178606</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B24" t="str">
         <f>table2_calc!F16</f>
         <v>Non-Hispanic Black</v>
@@ -3450,7 +3630,7 @@
         <v>0.21814224857765444</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B25" t="str">
         <f>table2_calc!F17</f>
         <v>Non-Hispanic White</v>
@@ -3460,7 +3640,7 @@
         <v>0.16864340763245622</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B26" t="str">
         <f>table2_calc!F18</f>
         <v>Other Hispanic</v>
@@ -3470,7 +3650,7 @@
         <v>0.17783260080896857</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B27" t="str">
         <f>table2_calc!F19</f>
         <v>Other Race - Including Multi-Racial</v>
@@ -3480,7 +3660,7 @@
         <v>0.11155327777253495</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>110</v>
       </c>
@@ -3489,7 +3669,7 @@
         <v>&lt;0.0001</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B29" t="str">
         <f>table2_calc!F20</f>
         <v>20-24</v>
@@ -3499,7 +3679,7 @@
         <v>0.11617941932736178</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B30" t="str">
         <f>table2_calc!F21</f>
         <v>25-29</v>
@@ -3509,7 +3689,7 @@
         <v>0.13802863792458381</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B31" t="str">
         <f>table2_calc!F22</f>
         <v>30-34</v>
@@ -3519,7 +3699,7 @@
         <v>0.14866502836122775</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B32" t="str">
         <f>table2_calc!F23</f>
         <v>35-39</v>
@@ -3529,7 +3709,7 @@
         <v>0.15005803473066776</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B33" t="str">
         <f>table2_calc!F24</f>
         <v>40-44</v>
@@ -3539,7 +3719,7 @@
         <v>0.17220187687542327</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B34" t="str">
         <f>table2_calc!F25</f>
         <v>45-49</v>
@@ -3549,7 +3729,7 @@
         <v>0.18520774825067401</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B35" t="str">
         <f>table2_calc!F26</f>
         <v>50-54</v>
@@ -3559,7 +3739,7 @@
         <v>0.18126970937797615</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B36" t="str">
         <f>table2_calc!F27</f>
         <v>55-59</v>
@@ -3569,7 +3749,7 @@
         <v>0.19051478290084661</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B37" t="str">
         <f>table2_calc!F28</f>
         <v>60-64</v>
@@ -3579,7 +3759,7 @@
         <v>0.22206908142089243</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B38" t="str">
         <f>table2_calc!F29</f>
         <v>65-69</v>
@@ -3589,7 +3769,7 @@
         <v>0.21111759522832091</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B39" t="str">
         <f>table2_calc!F30</f>
         <v>70-74</v>
@@ -3599,7 +3779,7 @@
         <v>0.2257345194460558</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B40" t="str">
         <f>table2_calc!F31</f>
         <v>75-79</v>
@@ -3609,7 +3789,7 @@
         <v>0.2132110812163136</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B41" t="str">
         <f>table2_calc!F32</f>
         <v>80+</v>
@@ -3619,7 +3799,7 @@
         <v>0.21366831476845946</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>111</v>
       </c>
@@ -3628,7 +3808,7 @@
         <v>&lt;0.0001</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B43" t="str">
         <f>table2_calc!F33</f>
         <v>Missing</v>
@@ -3638,7 +3818,7 @@
         <v>0.18155186948093988</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B44" t="str">
         <f>table2_calc!F34</f>
         <v>N/A (Male)</v>
@@ -3648,7 +3828,7 @@
         <v>0.14851840777308084</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B45" t="str">
         <f>table2_calc!F35</f>
         <v>No</v>
@@ -3658,7 +3838,7 @@
         <v>0.1905848975528118</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B46" t="str">
         <f>table2_calc!F36</f>
         <v>Yes</v>
@@ -3668,7 +3848,7 @@
         <v>0.29924453419234082</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>112</v>
       </c>
@@ -3677,7 +3857,7 @@
         <v>&lt;0.0001</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B48" t="str">
         <f>table2_calc!F37</f>
         <v>3+ ng/mL</v>
@@ -3687,7 +3867,7 @@
         <v>0.17793435598692231</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B49" t="str">
         <f>table2_calc!F38</f>
         <v>&lt;3 ng/mL</v>
@@ -3697,7 +3877,7 @@
         <v>0.16935347540341122</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>76</v>
       </c>
@@ -3706,7 +3886,7 @@
         <v>&lt;0.0001</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B51" t="str">
         <f>table2_calc!F39</f>
         <v>Missing</v>
@@ -3716,7 +3896,7 @@
         <v>0.18578159144309772</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B52" t="str">
         <f>table2_calc!F40</f>
         <v>N/A (Male)</v>
@@ -3726,7 +3906,7 @@
         <v>0.14851840777308084</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B53" t="str">
         <f>table2_calc!F41</f>
         <v>No</v>
@@ -3736,7 +3916,7 @@
         <v>0.19490757069347936</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B54" t="str">
         <f>table2_calc!F42</f>
         <v>Yes</v>
@@ -3746,7 +3926,7 @@
         <v>0.29825981522626099</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>113</v>
       </c>
@@ -3755,7 +3935,7 @@
         <v>&lt;0.0001</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B56" t="str">
         <f>table2_calc!F43</f>
         <v>No</v>
@@ -3765,7 +3945,7 @@
         <v>0.12033979052935298</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B57" t="str">
         <f>table2_calc!F44</f>
         <v>Yes</v>
@@ -3775,7 +3955,7 @@
         <v>0.34050663658668029</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>80</v>
       </c>
@@ -3784,7 +3964,7 @@
         <v>&lt;0.0001</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B59" t="str">
         <f>table2_calc!F45</f>
         <v>No</v>
@@ -3794,7 +3974,7 @@
         <v>0.16408092878777195</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B60" t="str">
         <f>table2_calc!F46</f>
         <v>Yes</v>
@@ -3804,7 +3984,7 @@
         <v>0.17956541613026039</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>114</v>
       </c>
@@ -3813,7 +3993,7 @@
         <v>&lt;0.0001</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B62" t="str">
         <f>table2_calc!F47</f>
         <v>No</v>
@@ -3823,7 +4003,7 @@
         <v>0.16700952555250428</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B63" t="str">
         <f>table2_calc!F48</f>
         <v>Yes</v>
@@ -3833,7 +4013,7 @@
         <v>0.20431568367807684</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>115</v>
       </c>
@@ -3842,7 +4022,7 @@
         <v>&lt;0.0001</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B65" t="str">
         <f>table2_calc!F49</f>
         <v>Missing</v>
@@ -3852,7 +4032,7 @@
         <v>0.25192380084514909</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="5"/>
       <c r="B66" s="5" t="str">
         <f>table2_calc!F50</f>
@@ -3864,21 +4044,21 @@
       </c>
       <c r="D66" s="25"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="4"/>
       <c r="B67" s="4" t="str">
         <f>table2_calc!F51</f>
         <v>Yes</v>
       </c>
-      <c r="C67" s="34">
+      <c r="C67" s="27">
         <f>table2_calc!E51</f>
         <v>0.19018583401562669</v>
       </c>
-      <c r="D67" s="35"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D67" s="28"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -3899,13 +4079,13 @@
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>84</v>
       </c>
@@ -3922,7 +4102,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -3939,11 +4119,11 @@
         <v>0.20597082564191388</v>
       </c>
       <c r="F2" t="str">
-        <f>SUBSTITUTE(B2,A2&amp;" ","")</f>
+        <f t="shared" ref="F2:F33" si="0">SUBSTITUTE(B2,A2&amp;" ","")</f>
         <v>9-11th Grade (Includes 12th grade with no diploma)</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -3960,11 +4140,11 @@
         <v>0.1324012443088248</v>
       </c>
       <c r="F3" t="str">
-        <f>SUBSTITUTE(B3,A3&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>College Graduate or above</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -3981,11 +4161,11 @@
         <v>0.19382391348629144</v>
       </c>
       <c r="F4" t="str">
-        <f>SUBSTITUTE(B4,A4&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>High School Grad/GED or Equivalent</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -4002,11 +4182,11 @@
         <v>0.2038299658849701</v>
       </c>
       <c r="F5" t="str">
-        <f>SUBSTITUTE(B5,A5&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>Less Than 9th Grade</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -4023,11 +4203,11 @@
         <v>0.17491922473584842</v>
       </c>
       <c r="F6" t="str">
-        <f>SUBSTITUTE(B6,A6&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>Some College or AA degree</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -4044,11 +4224,11 @@
         <v>0.19378954272376392</v>
       </c>
       <c r="F7" t="str">
-        <f>SUBSTITUTE(B7,A7&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>0-100%</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -4065,11 +4245,11 @@
         <v>0.19351952704729519</v>
       </c>
       <c r="F8" t="str">
-        <f>SUBSTITUTE(B8,A8&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>100-199%</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -4086,11 +4266,11 @@
         <v>0.15984129219753143</v>
       </c>
       <c r="F9" t="str">
-        <f>SUBSTITUTE(B9,A9&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>200%+</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -4107,11 +4287,11 @@
         <v>0.18428802217283879</v>
       </c>
       <c r="F10" t="str">
-        <f>SUBSTITUTE(B10,A10&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>Missing</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -4128,11 +4308,11 @@
         <v>0.23397085117818919</v>
       </c>
       <c r="F11" t="str">
-        <f>SUBSTITUTE(B11,A11&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>No</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -4149,11 +4329,11 @@
         <v>0.1497332017604846</v>
       </c>
       <c r="F12" t="str">
-        <f>SUBSTITUTE(B12,A12&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -4170,11 +4350,11 @@
         <v>0.19724557055808828</v>
       </c>
       <c r="F13" t="str">
-        <f>SUBSTITUTE(B13,A13&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>Female</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -4191,11 +4371,11 @@
         <v>0.14851840777308084</v>
       </c>
       <c r="F14" t="str">
-        <f>SUBSTITUTE(B14,A14&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>Male</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -4212,11 +4392,11 @@
         <v>0.19827848213178606</v>
       </c>
       <c r="F15" t="str">
-        <f>SUBSTITUTE(B15,A15&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>Mexican American</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -4233,11 +4413,11 @@
         <v>0.21814224857765444</v>
       </c>
       <c r="F16" t="str">
-        <f>SUBSTITUTE(B16,A16&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>Non-Hispanic Black</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -4254,11 +4434,11 @@
         <v>0.16864340763245622</v>
       </c>
       <c r="F17" t="str">
-        <f>SUBSTITUTE(B17,A17&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>Non-Hispanic White</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -4275,11 +4455,11 @@
         <v>0.17783260080896857</v>
       </c>
       <c r="F18" t="str">
-        <f>SUBSTITUTE(B18,A18&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>Other Hispanic</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -4296,11 +4476,11 @@
         <v>0.11155327777253495</v>
       </c>
       <c r="F19" t="str">
-        <f>SUBSTITUTE(B19,A19&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>Other Race - Including Multi-Racial</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>89</v>
       </c>
@@ -4317,11 +4497,11 @@
         <v>0.11617941932736178</v>
       </c>
       <c r="F20" t="str">
-        <f>SUBSTITUTE(B20,A20&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>20-24</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>89</v>
       </c>
@@ -4338,11 +4518,11 @@
         <v>0.13802863792458381</v>
       </c>
       <c r="F21" t="str">
-        <f>SUBSTITUTE(B21,A21&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>25-29</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>89</v>
       </c>
@@ -4359,11 +4539,11 @@
         <v>0.14866502836122775</v>
       </c>
       <c r="F22" t="str">
-        <f>SUBSTITUTE(B22,A22&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>30-34</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -4380,11 +4560,11 @@
         <v>0.15005803473066776</v>
       </c>
       <c r="F23" t="str">
-        <f>SUBSTITUTE(B23,A23&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>35-39</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>89</v>
       </c>
@@ -4401,11 +4581,11 @@
         <v>0.17220187687542327</v>
       </c>
       <c r="F24" t="str">
-        <f>SUBSTITUTE(B24,A24&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>40-44</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>89</v>
       </c>
@@ -4422,11 +4602,11 @@
         <v>0.18520774825067401</v>
       </c>
       <c r="F25" t="str">
-        <f>SUBSTITUTE(B25,A25&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>45-49</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>89</v>
       </c>
@@ -4443,11 +4623,11 @@
         <v>0.18126970937797615</v>
       </c>
       <c r="F26" t="str">
-        <f>SUBSTITUTE(B26,A26&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>50-54</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>89</v>
       </c>
@@ -4464,11 +4644,11 @@
         <v>0.19051478290084661</v>
       </c>
       <c r="F27" t="str">
-        <f>SUBSTITUTE(B27,A27&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>55-59</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>89</v>
       </c>
@@ -4485,11 +4665,11 @@
         <v>0.22206908142089243</v>
       </c>
       <c r="F28" t="str">
-        <f>SUBSTITUTE(B28,A28&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>60-64</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>89</v>
       </c>
@@ -4506,11 +4686,11 @@
         <v>0.21111759522832091</v>
       </c>
       <c r="F29" t="str">
-        <f>SUBSTITUTE(B29,A29&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>65-69</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>89</v>
       </c>
@@ -4527,11 +4707,11 @@
         <v>0.2257345194460558</v>
       </c>
       <c r="F30" t="str">
-        <f>SUBSTITUTE(B30,A30&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>70-74</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>89</v>
       </c>
@@ -4548,11 +4728,11 @@
         <v>0.2132110812163136</v>
       </c>
       <c r="F31" t="str">
-        <f>SUBSTITUTE(B31,A31&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>75-79</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>89</v>
       </c>
@@ -4569,11 +4749,11 @@
         <v>0.21366831476845946</v>
       </c>
       <c r="F32" t="str">
-        <f>SUBSTITUTE(B32,A32&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>80+</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>140</v>
       </c>
@@ -4590,11 +4770,11 @@
         <v>0.18155186948093988</v>
       </c>
       <c r="F33" t="str">
-        <f>SUBSTITUTE(B33,A33&amp;" ","")</f>
+        <f t="shared" si="0"/>
         <v>Missing</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>140</v>
       </c>
@@ -4611,11 +4791,11 @@
         <v>0.14851840777308084</v>
       </c>
       <c r="F34" t="str">
-        <f>SUBSTITUTE(B34,A34&amp;" ","")</f>
+        <f t="shared" ref="F34:F51" si="1">SUBSTITUTE(B34,A34&amp;" ","")</f>
         <v>N/A (Male)</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>140</v>
       </c>
@@ -4632,11 +4812,11 @@
         <v>0.1905848975528118</v>
       </c>
       <c r="F35" t="str">
-        <f>SUBSTITUTE(B35,A35&amp;" ","")</f>
+        <f t="shared" si="1"/>
         <v>No</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>140</v>
       </c>
@@ -4653,11 +4833,11 @@
         <v>0.29924453419234082</v>
       </c>
       <c r="F36" t="str">
-        <f>SUBSTITUTE(B36,A36&amp;" ","")</f>
+        <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>141</v>
       </c>
@@ -4674,11 +4854,11 @@
         <v>0.17793435598692231</v>
       </c>
       <c r="F37" t="str">
-        <f>SUBSTITUTE(B37,A37&amp;" ","")</f>
+        <f t="shared" si="1"/>
         <v>3+ ng/mL</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>141</v>
       </c>
@@ -4695,11 +4875,11 @@
         <v>0.16935347540341122</v>
       </c>
       <c r="F38" t="str">
-        <f>SUBSTITUTE(B38,A38&amp;" ","")</f>
+        <f t="shared" si="1"/>
         <v>&lt;3 ng/mL</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>59</v>
       </c>
@@ -4716,11 +4896,11 @@
         <v>0.18578159144309772</v>
       </c>
       <c r="F39" t="str">
-        <f>SUBSTITUTE(B39,A39&amp;" ","")</f>
+        <f t="shared" si="1"/>
         <v>Missing</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>59</v>
       </c>
@@ -4737,11 +4917,11 @@
         <v>0.14851840777308084</v>
       </c>
       <c r="F40" t="str">
-        <f>SUBSTITUTE(B40,A40&amp;" ","")</f>
+        <f t="shared" si="1"/>
         <v>N/A (Male)</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>59</v>
       </c>
@@ -4758,11 +4938,11 @@
         <v>0.19490757069347936</v>
       </c>
       <c r="F41" t="str">
-        <f>SUBSTITUTE(B41,A41&amp;" ","")</f>
+        <f t="shared" si="1"/>
         <v>No</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>59</v>
       </c>
@@ -4779,11 +4959,11 @@
         <v>0.29825981522626099</v>
       </c>
       <c r="F42" t="str">
-        <f>SUBSTITUTE(B42,A42&amp;" ","")</f>
+        <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>60</v>
       </c>
@@ -4800,11 +4980,11 @@
         <v>0.12033979052935298</v>
       </c>
       <c r="F43" t="str">
-        <f>SUBSTITUTE(B43,A43&amp;" ","")</f>
+        <f t="shared" si="1"/>
         <v>No</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>60</v>
       </c>
@@ -4821,11 +5001,11 @@
         <v>0.34050663658668029</v>
       </c>
       <c r="F44" t="str">
-        <f>SUBSTITUTE(B44,A44&amp;" ","")</f>
+        <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>142</v>
       </c>
@@ -4842,11 +5022,11 @@
         <v>0.16408092878777195</v>
       </c>
       <c r="F45" t="str">
-        <f>SUBSTITUTE(B45,A45&amp;" ","")</f>
+        <f t="shared" si="1"/>
         <v>No</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>142</v>
       </c>
@@ -4863,11 +5043,11 @@
         <v>0.17956541613026039</v>
       </c>
       <c r="F46" t="str">
-        <f>SUBSTITUTE(B46,A46&amp;" ","")</f>
+        <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>143</v>
       </c>
@@ -4884,11 +5064,11 @@
         <v>0.16700952555250428</v>
       </c>
       <c r="F47" t="str">
-        <f>SUBSTITUTE(B47,A47&amp;" ","")</f>
+        <f t="shared" si="1"/>
         <v>No</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>143</v>
       </c>
@@ -4905,11 +5085,11 @@
         <v>0.20431568367807684</v>
       </c>
       <c r="F48" t="str">
-        <f>SUBSTITUTE(B48,A48&amp;" ","")</f>
+        <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>144</v>
       </c>
@@ -4926,11 +5106,11 @@
         <v>0.25192380084514909</v>
       </c>
       <c r="F49" t="str">
-        <f>SUBSTITUTE(B49,A49&amp;" ","")</f>
+        <f t="shared" si="1"/>
         <v>Missing</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>144</v>
       </c>
@@ -4947,11 +5127,11 @@
         <v>0.16769054523312726</v>
       </c>
       <c r="F50" t="str">
-        <f>SUBSTITUTE(B50,A50&amp;" ","")</f>
+        <f t="shared" si="1"/>
         <v>No</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>144</v>
       </c>
@@ -4968,7 +5148,7 @@
         <v>0.19018583401562669</v>
       </c>
       <c r="F51" t="str">
-        <f>SUBSTITUTE(B51,A51&amp;" ","")</f>
+        <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
     </row>
@@ -4982,61 +5162,61 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="J17" sqref="A1:J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" customWidth="1"/>
-    <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.81640625" customWidth="1"/>
+    <col min="2" max="2" width="7.1796875" customWidth="1"/>
+    <col min="3" max="3" width="13.26953125" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" customWidth="1"/>
+    <col min="7" max="7" width="6.7265625" customWidth="1"/>
+    <col min="8" max="8" width="6.453125" customWidth="1"/>
+    <col min="9" max="9" width="5.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:10" ht="45.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-    </row>
-    <row r="2" spans="1:10" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="29" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+    </row>
+    <row r="2" spans="1:10" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-    </row>
-    <row r="3" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+    </row>
+    <row r="3" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32" t="s">
+      <c r="H3" s="36"/>
+      <c r="I3" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="J3" s="32"/>
-    </row>
-    <row r="4" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="36"/>
+    </row>
+    <row r="4" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C4" s="20" t="s">
         <v>124</v>
       </c>
@@ -5062,12 +5242,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -5104,7 +5284,7 @@
         <v>1.00--1.02</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -5141,7 +5321,7 @@
         <v>1.00--1.01</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -5170,12 +5350,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -5204,7 +5384,7 @@
         <v>0.98--1.00</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>5</v>
       </c>
@@ -5233,7 +5413,7 @@
         <v>0.98--1.00</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>6</v>
       </c>
@@ -5262,7 +5442,7 @@
         <v>0.98--1.00</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>8</v>
       </c>
@@ -5291,7 +5471,7 @@
         <v>0.98--1.00</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="5" t="s">
         <v>9</v>
@@ -5317,7 +5497,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="E15" s="7"/>
@@ -5328,20 +5508,20 @@
       <c r="J15" s="7"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -5361,18 +5541,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="42.140625" customWidth="1"/>
+    <col min="1" max="1" width="42.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5413,7 +5593,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -5445,7 +5625,7 @@
         <v>0.25541720318323613</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -5468,7 +5648,7 @@
         <v>-0.1998525767472446</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -5500,7 +5680,7 @@
         <v>0.17802830072023007</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -5532,7 +5712,7 @@
         <v>0.23870796935333638</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -5564,7 +5744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -5605,7 +5785,7 @@
         <v>0.25700250696301019</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -5646,7 +5826,7 @@
         <v>0.2661738402223558</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -5669,7 +5849,316 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="14.45" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.6328125" customWidth="1"/>
+    <col min="2" max="2" width="5.36328125" customWidth="1"/>
+    <col min="3" max="3" width="1.6328125" customWidth="1"/>
+    <col min="4" max="4" width="5.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" customWidth="1"/>
+    <col min="6" max="6" width="4.7265625" customWidth="1"/>
+    <col min="7" max="7" width="1.90625" customWidth="1"/>
+    <col min="8" max="8" width="4.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+    </row>
+    <row r="2" spans="1:9" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="39"/>
+      <c r="B2" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.35">
+      <c r="A3" s="39"/>
+      <c r="B3" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="41"/>
+      <c r="D3" s="42" t="s">
+        <v>158</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="F3" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="G3" s="41"/>
+      <c r="H3" s="42" t="s">
+        <v>158</v>
+      </c>
+      <c r="I3" s="43" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="44">
+        <f>suppl_tbl1_calc!B2</f>
+        <v>78.693606161206347</v>
+      </c>
+      <c r="C4" s="44"/>
+      <c r="D4" s="39">
+        <f>suppl_tbl1_calc!C2</f>
+        <v>4</v>
+      </c>
+      <c r="E4" s="45" t="str">
+        <f>IF(suppl_tbl1_calc!D2&lt;0.0001,"&lt;0.0001",suppl_tbl1_calc!D2)</f>
+        <v>&lt;0.0001</v>
+      </c>
+      <c r="F4" s="44">
+        <f>suppl_tbl1_calc!E2</f>
+        <v>4.615773777175332</v>
+      </c>
+      <c r="G4" s="44"/>
+      <c r="H4" s="39">
+        <f>suppl_tbl1_calc!F2</f>
+        <v>4</v>
+      </c>
+      <c r="I4" s="46">
+        <f>IF(suppl_tbl1_calc!G2&lt;0.0001,"&lt;0.0001",suppl_tbl1_calc!G2)</f>
+        <v>0.32903955571615162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="44">
+        <f>suppl_tbl1_calc!B4</f>
+        <v>59.219320172711321</v>
+      </c>
+      <c r="C5" s="44"/>
+      <c r="D5" s="39">
+        <f>suppl_tbl1_calc!C4</f>
+        <v>2</v>
+      </c>
+      <c r="E5" s="45" t="str">
+        <f>IF(suppl_tbl1_calc!D4&lt;0.0001,"&lt;0.0001",suppl_tbl1_calc!D4)</f>
+        <v>&lt;0.0001</v>
+      </c>
+      <c r="F5" s="44">
+        <f>suppl_tbl1_calc!E4</f>
+        <v>11.578927707897538</v>
+      </c>
+      <c r="G5" s="44"/>
+      <c r="H5" s="39">
+        <f>suppl_tbl1_calc!F4</f>
+        <v>2</v>
+      </c>
+      <c r="I5" s="45">
+        <f>IF(suppl_tbl1_calc!G4&lt;0.0001,"&lt;0.0001",suppl_tbl1_calc!G4)</f>
+        <v>3.0596221410829402E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="47" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" s="48">
+        <f>suppl_tbl1_calc!B3</f>
+        <v>6.4495012723888756</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" s="47">
+        <f>suppl_tbl1_calc!C3</f>
+        <v>1</v>
+      </c>
+      <c r="E6" s="49">
+        <f>IF(suppl_tbl1_calc!D3&lt;0.0001,"&lt;0.0001",suppl_tbl1_calc!D3)</f>
+        <v>1.4465265919984651E-2</v>
+      </c>
+      <c r="F6" s="48">
+        <f>suppl_tbl1_calc!E3</f>
+        <v>5.1455183930930355</v>
+      </c>
+      <c r="G6" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="H6" s="47">
+        <f>suppl_tbl1_calc!F3</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="49">
+        <f>IF(suppl_tbl1_calc!G3&lt;0.0001,"&lt;0.0001",suppl_tbl1_calc!G3)</f>
+        <v>2.7941983038578536E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="5.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="50"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.35">
+      <c r="A8" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2">
+        <v>78.693606161206347</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>3.2938943874834198E-16</v>
+      </c>
+      <c r="E2">
+        <v>4.615773777175332</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>0.32903955571615162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3">
+        <v>6.4495012723888756</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1.4465265919984651E-2</v>
+      </c>
+      <c r="E3">
+        <v>5.1455183930930355</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2.7941983038578536E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4">
+        <v>59.219320172711321</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1.382572815638457E-13</v>
+      </c>
+      <c r="E4">
+        <v>11.578927707897538</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>3.0596221410829402E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>